<commit_message>
fix: Improve tier table reading and partial fill handling
- Fix tier table row range (23-262) in excel_bridge.py
- Add Tier 230/240 risk warnings in grid_engine.py
- Enhance batch order partial fill handling
- Add zero division protection in quantity calculations
- Auto-calculate tier amount (B6) when empty or formula
- Clean up Claude permissions settings

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/phoenix_grid_template_v3.xlsx
+++ b/phoenix_grid_template_v3.xlsx
@@ -574,10 +574,9 @@
           <t>1티어 금액 (USD)</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>500</t>
-        </is>
+      <c r="B6">
+        <f>B4/B5</f>
+        <v/>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -670,11 +669,6 @@
           <t>KIS APP KEY</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>your_kis_app_key_here</t>
-        </is>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -710,12 +704,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16"/>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>시세 조회 주기 (초)</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>40</v>
+      </c>
+    </row>
     <row r="17">
       <c r="A17" s="1">
         <f>== 텔레그램 알림 ===</f>
         <v/>
       </c>
+      <c r="B17" t="n">
+        <v>500</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -730,6 +736,9 @@
           <t>텔레그램 Token</t>
         </is>
       </c>
+      <c r="B19" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -737,10 +746,8 @@
           <t>알림 활성화</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>FALSE</t>
-        </is>
+      <c r="B20" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -749,10 +756,8 @@
           <t>Excel 업데이트 주기 (초)</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>40.0</t>
-        </is>
+      <c r="B21" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="22">
@@ -761,10 +766,8 @@
           <t>티어</t>
         </is>
       </c>
-      <c r="B22" s="2" t="inlineStr">
-        <is>
-          <t>시드비%</t>
-        </is>
+      <c r="B22" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="C22" s="2" t="inlineStr">
         <is>

</xml_diff>